<commit_message>
confirmation duplikáció fix + kis egyéb fixek
</commit_message>
<xml_diff>
--- a/back tests.xlsx
+++ b/back tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -93,6 +93,9 @@
     <t xml:space="preserve">Pass</t>
   </si>
   <si>
+    <t xml:space="preserve">SP-2,SP-10,SP-11</t>
+  </si>
+  <si>
     <t xml:space="preserve">SP-2</t>
   </si>
   <si>
@@ -118,6 +121,9 @@
     <t xml:space="preserve">Response: 200 (OK), body: „email_kuldve" Creates a new confirmation, and sends an email</t>
   </si>
   <si>
+    <t xml:space="preserve">SP-12</t>
+  </si>
+  <si>
     <t xml:space="preserve">SP-4</t>
   </si>
   <si>
@@ -130,6 +136,9 @@
     <t xml:space="preserve">Response: 200 (OK), body: „jelszo_megvaltoztatva" Changes the user's password, deletes confirmation</t>
   </si>
   <si>
+    <t xml:space="preserve">SP-15,SP-16</t>
+  </si>
+  <si>
     <t xml:space="preserve">SP-5</t>
   </si>
   <si>
@@ -142,6 +151,9 @@
     <t xml:space="preserve">Response: 200 (OK), body: „email kuldve" Sends email </t>
   </si>
   <si>
+    <t xml:space="preserve">SP-13</t>
+  </si>
+  <si>
     <t xml:space="preserve">SP-6</t>
   </si>
   <si>
@@ -151,6 +163,9 @@
     <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/delacc_request/ with the body  „ {    "id": "&lt;b64encoded id”, "password": "&lt;b64 encoded password_hash&gt;" } </t>
   </si>
   <si>
+    <t xml:space="preserve">SP-14</t>
+  </si>
+  <si>
     <t xml:space="preserve">SP-7</t>
   </si>
   <si>
@@ -175,12 +190,6 @@
     <t xml:space="preserve">It adds 33 test users</t>
   </si>
   <si>
-    <t xml:space="preserve">SP-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.02.2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">SP-10</t>
   </si>
   <si>
@@ -188,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „felhasznalo_mar_letezik”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-1,SP-11</t>
   </si>
   <si>
     <t xml:space="preserve">SP-11</t>
@@ -231,7 +243,7 @@
     <t xml:space="preserve">Response: 400 (BAD REQUEST), body: „hibas_request”</t>
   </si>
   <si>
-    <t xml:space="preserve">SP-12</t>
+    <t xml:space="preserve">SP-1,SP-10</t>
   </si>
   <si>
     <t xml:space="preserve">Test if api/chpass_request works (with a nonexisting user)</t>
@@ -243,18 +255,12 @@
     <t xml:space="preserve">Response: 500 (OK), body: „sze_v_felhasznalo_nem_letezik"</t>
   </si>
   <si>
-    <t xml:space="preserve">SP-13</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test if api/login works (wrong password)</t>
   </si>
   <si>
     <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hibas_jelszo" Sends email </t>
   </si>
   <si>
-    <t xml:space="preserve">SP-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test if api/delacc_request works (with a nonexisting user)</t>
   </si>
   <si>
@@ -267,6 +273,9 @@
     <t xml:space="preserve">Response: 400 (BAD REQUEST), body: „hibas_token"</t>
   </si>
   <si>
+    <t xml:space="preserve">SP-4,SP-16</t>
+  </si>
+  <si>
     <t xml:space="preserve">12.16.2025</t>
   </si>
   <si>
@@ -279,6 +288,9 @@
     <t xml:space="preserve">Response: 404 (NOT FOUND), body: „confirmation_nem_letezik_vagy_hibas"</t>
   </si>
   <si>
+    <t xml:space="preserve">SP-4,SP-15</t>
+  </si>
+  <si>
     <t xml:space="preserve">SP-17</t>
   </si>
   <si>
@@ -286,6 +298,81 @@
   </si>
   <si>
     <t xml:space="preserve">Response: 410 (GONE), body: „confirmation_lejart"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if add_test_products works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Click add products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It adds 33 test products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if add_test_orders works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Click add test orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It adds 33 test orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/registration_promise works (wrong token)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    "id": "&lt;b64encoded user_id”, "token": "&lt;wrong b64 encoded confirmation_token&gt;" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hibas_token"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-2,SP-10,SP-11,SP-21,SP-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.01.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/registration_promise works (user already activated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 409 (CONFLICT), body: „felhasznalo_mar_aktivalva"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/registration_promise works (wrong/nonexistent id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    "id": "&lt;b64encoded user_id”, "token": "&lt;random b64 encoded confirmation_token&gt;" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 404 (NOT FOUND), body: „felhasznalo_nem_letezik"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-2,SP-10,SP-11,SP-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-2,SP-10,SP-11,SP-22</t>
   </si>
 </sst>
 </file>
@@ -351,7 +438,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,6 +475,12 @@
         <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -423,7 +516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,6 +575,18 @@
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -733,10 +838,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,25 +921,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="I3" s="11" t="n">
         <v>45979</v>
@@ -845,25 +947,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I4" s="11" t="n">
         <v>45979</v>
@@ -874,25 +976,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I5" s="11" t="n">
         <v>45979</v>
@@ -903,22 +1005,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>13</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I6" s="11" t="n">
         <v>45980</v>
@@ -929,25 +1034,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="F7" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
+      <c r="H7" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="I7" s="11" t="n">
         <v>45980</v>
@@ -958,25 +1063,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="I8" s="11" t="n">
         <v>45982</v>
@@ -987,19 +1092,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>13</v>
@@ -1009,58 +1114,37 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>42</v>
-      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="I11" s="11" t="n">
         <v>46005</v>
@@ -1071,25 +1155,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="I12" s="11" t="n">
         <v>46005</v>
@@ -1100,25 +1184,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I13" s="11" t="n">
         <v>46006</v>
@@ -1129,25 +1213,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I14" s="11" t="n">
         <v>46006</v>
@@ -1158,141 +1242,287 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="F15" s="9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I15" s="11" t="n">
         <v>46006</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="34.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="34.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="11" t="n">
+        <v>46034</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="11" t="n">
+        <v>46034</v>
+      </c>
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C20" s="12"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C21" s="12"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C22" s="12"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C23" s="12"/>
+      <c r="B23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    &quot;id&quot;: &quot;&lt;b64encoded user_id”, &quot;token&quot;: &quot;&lt;b64 encoded confirmation_token&gt;&quot; }"/>
-    <hyperlink ref="D7" r:id="rId2" display="1. Open postman 2. Send a request to  http://localhost:90/api/delacc_request/ with the body  „ {    &quot;id&quot;: &quot;&lt;b64encoded id”, &quot;password&quot;: &quot;&lt;b64 encoded password_hash&gt;&quot; } "/>
-    <hyperlink ref="D15" r:id="rId3" display="1. Open postman 2. Send a request to  http://localhost:90/api/delacc_request/ with the body  „ {    &quot;id&quot;: &quot;&lt;b64encoded id”, &quot;password&quot;: &quot;&lt;b64 encoded password_hash&gt;&quot; } "/>
-    <hyperlink ref="D16" r:id="rId4" display="1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    &quot;id&quot;: &quot;&lt;b64encoded user_id”, &quot;token&quot;: &quot;&lt;b64 encoded confirmation_token&gt;&quot; }"/>
-    <hyperlink ref="D17" r:id="rId5" display="1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    &quot;id&quot;: &quot;&lt;b64encoded user_id”, &quot;token&quot;: &quot;&lt;b64 encoded confirmation_token&gt;&quot; }"/>
-    <hyperlink ref="D18" r:id="rId6" display="1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    &quot;id&quot;: &quot;&lt;b64encoded user_id”, &quot;token&quot;: &quot;&lt;b64 encoded confirmation_token&gt;&quot; }"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
jwt nem ellenőrzi a token-t fix, szerver nem indul el mert nem tud portot foglalni fix
</commit_message>
<xml_diff>
--- a/back tests.xlsx
+++ b/back tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="174">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -58,7 +58,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -68,7 +68,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="238"/>
@@ -78,7 +78,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/delacc_request/ with the body  „ {    "id": "&lt;b64encoded id”, "password": "&lt;b64 encoded password_hash&gt;" } </t>
   </si>
   <si>
-    <t xml:space="preserve">TI-14</t>
+    <t xml:space="preserve">TI-14,T-38</t>
   </si>
   <si>
     <t xml:space="preserve">TI-7</t>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">Response: 200 (OK), body: „felhasznalo_torolve" Deletes account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-6,T-39</t>
   </si>
   <si>
     <t xml:space="preserve">TI-8</t>
@@ -223,7 +226,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -233,7 +236,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="238"/>
@@ -243,7 +246,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -273,9 +276,15 @@
     <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hibas_jelszo" Sends email </t>
   </si>
   <si>
+    <t xml:space="preserve">TI-14</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test if api/delacc_request works (with a nonexisting user)</t>
   </si>
   <si>
+    <t xml:space="preserve">TI-6,T-38</t>
+  </si>
+  <si>
     <t xml:space="preserve">TI-15</t>
   </si>
   <si>
@@ -285,7 +294,7 @@
     <t xml:space="preserve">Response: 400 (BAD REQUEST), body: „hibas_token"</t>
   </si>
   <si>
-    <t xml:space="preserve">TI-4,TI-16</t>
+    <t xml:space="preserve">TI-4,TI-16,T-39</t>
   </si>
   <si>
     <t xml:space="preserve">12.16.2025</t>
@@ -315,7 +324,7 @@
     <t xml:space="preserve">TI-18</t>
   </si>
   <si>
-    <t xml:space="preserve">Test if add_test_products works</t>
+    <t xml:space="preserve">Test if add_test_products works  (test panel)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Open the Test panel 2. Click add products</t>
@@ -327,109 +336,271 @@
     <t xml:space="preserve">TI-19</t>
   </si>
   <si>
+    <t xml:space="preserve">Test if add_test_orders works (test panel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Click add test orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It adds 33 test orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/registration_promise works (wrong token)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    "id": "&lt;b64encoded user_id”, "token": "&lt;wrong b64 encoded confirmation_token&gt;" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hibas_token"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-2,TI-10,TI-11,TI-21,TI-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.01.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/registration_promise works (user already activated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 409 (CONFLICT), body: „felhasznalo_mar_aktivalva"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/registration_promise works (wrong/nonexistent id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    "id": "&lt;b64encoded user_id”, "token": "&lt;random b64 encoded confirmation_token&gt;" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 404 (NOT FOUND), body: „felhasznalo_nem_letezik"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-2,TI-10,TI-11,TI-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-2,TI-10,TI-11,TI-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if add test confirmations (test panel) works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Click the add test confirmations button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It adds 33 test confirmations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-25, T-32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if delete all confirmations (test panel) works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Click the delete all confirmations button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It deletes all existing confirmations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-24, T-32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if delete all products (test panel) works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Click the delete all products button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It deletes all existing products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if delet all orders (test panel) works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Click the delete all orders button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if add test product images works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Type in the product id 3. Click the add test prod. Image button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It adds 3 test product images to the right product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if delete all test product images works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Click the delete all test prod. Image button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It deletes all existing product images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-31</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test if add_test_orders works</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Open the Test panel 2. Click add test orders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It adds 33 test orders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test if api/registration_promise works (wrong token)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    "id": "&lt;b64encoded user_id”, "token": "&lt;wrong b64 encoded confirmation_token&gt;" }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hibas_token"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-2,TI-10,TI-11,TI-21,TI-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.01.2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test if api/registration_promise works (user already activated)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response: 409 (CONFLICT), body: „felhasznalo_mar_aktivalva"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test if api/registration_promise works (wrong/nonexistent id)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    "id": "&lt;b64encoded user_id”, "token": "&lt;random b64 encoded confirmation_token&gt;" }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response: 404 (NOT FOUND), body: „felhasznalo_nem_letezik"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-2,TI-10,TI-11,TI-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-2,TI-10,TI-11,TI-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test if add test confirmations (test panel) works</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open the Test panel 2. Click add test confirmations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It adds 33 test confirmations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test if delete all confirmations (test panel) works</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open the Test panel 2. Click delete all confirmations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It deletes all existing confirmations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test if delete all products (test panel) works</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open the Test panel 2. Click delete all products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It deletes all existing products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI-27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test if delet all orders (test panel) works</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open the Test panel 2. Click delete all orders</t>
+    <t xml:space="preserve">1. Open the Test panel 2. Type in the user id 3. Click the add test orders button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It adds 33 test orders to the correct user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Type in the start user id (the id of the first user, the first out of 33 users with consequent user id’s) 3. Click the add test confirmations button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It adds 33 test confirmations to 33 different users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI-25, T-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if add test reviews (test panel) works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Type in the user id 3. Click the add test confirmations button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It adds 33 test reviews to the correct product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/get_all_products works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/get_all_products/ without a body and auth header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 200 (OK), body: „{ "statuscode": "200", "status": "no error", "products": [ «correctly formatted products here» ] }" (json response)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/chpass_promise/ with the body  „ {    "id": "&lt;b64encoded email”, "password": "&lt;b64 encoded password&gt;" } without an auth header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 200 (OK), body: „{ "token": "«token here»",  "expires_in": 604800 }" Sends email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/delacc_request/ with the body  „ {    "id": "&lt;b64encoded id”, "password": "&lt;b64 encoded password&gt;" } with an auth header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/delacc_promise/ with the body  „ {    "id": "&lt;b64encoded id”, "password": "&lt;b64 encoded token&gt;" } with an auth header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/delacc_request works (no auth header)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hianyzo_auth_header", Does not send the email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/delacc_promise works (no auth header)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hianyzo_auth_header", Didn’t delete the account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/delacc_request works (wrong or expired auth token in header)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hibas_token" Does not send the email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/delacc_promise works (wrong or expired auth token in header)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 401 (UNATHORIZED), body: „hibas_token" Did not delete account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if Test email (test panel) works </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Type in the email 3. Click the Test email button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It sends a test email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if Test magic link (test panel) works </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Test panel 2. Type in the email 3. Click the Test magic link button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It sends a test email with a specific code and displays that code in a textbox next to the email field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It doesn’t do anything</t>
   </si>
 </sst>
 </file>
@@ -440,7 +611,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,32 +638,46 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="238"/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color rgb="FF81D41A"/>
+      <name val="DejaVu Sans"/>
       <family val="2"/>
-      <charset val="238"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF81D41A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -511,7 +696,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor rgb="FF339966"/>
+        <bgColor rgb="FF81D41A"/>
       </patternFill>
     </fill>
     <fill>
@@ -573,36 +758,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,28 +791,56 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -687,7 +896,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFC55A11"/>
@@ -883,27 +1092,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="46.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="57.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="1" width="8.68"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -939,25 +1148,25 @@
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="11" t="n">
+      <c r="I2" s="9" t="n">
         <v>45978</v>
       </c>
     </row>
@@ -968,22 +1177,22 @@
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="11" t="n">
+      <c r="G3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="9" t="n">
         <v>45979</v>
       </c>
     </row>
@@ -994,25 +1203,25 @@
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="11" t="n">
+      <c r="I4" s="9" t="n">
         <v>45979</v>
       </c>
     </row>
@@ -1023,25 +1232,25 @@
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="11" t="n">
+      <c r="I5" s="9" t="n">
         <v>45979</v>
       </c>
     </row>
@@ -1052,25 +1261,25 @@
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="11" t="n">
+      <c r="I6" s="9" t="n">
         <v>45980</v>
       </c>
     </row>
@@ -1081,25 +1290,25 @@
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="11" t="n">
+      <c r="I7" s="9" t="n">
         <v>45980</v>
       </c>
     </row>
@@ -1110,25 +1319,25 @@
       <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="11" t="n">
+        <v>42</v>
+      </c>
+      <c r="I8" s="9" t="n">
         <v>45982</v>
       </c>
     </row>
@@ -1137,50 +1346,50 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="11" t="n">
+      <c r="E9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="9" t="n">
         <v>45982</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="24.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="11" t="n">
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="9" t="n">
         <v>45983</v>
       </c>
     </row>
@@ -1189,517 +1398,1114 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="11" t="n">
+        <v>54</v>
+      </c>
+      <c r="I11" s="9" t="n">
         <v>46005</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="60.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="E12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="11" t="n">
+        <v>59</v>
+      </c>
+      <c r="I12" s="9" t="n">
         <v>46005</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="57.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="F13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="11" t="n">
+      <c r="I13" s="9" t="n">
         <v>46006</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="E14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="11" t="n">
+      <c r="I14" s="9" t="n">
         <v>46006</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="57.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="E15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="11" t="n">
+        <v>67</v>
+      </c>
+      <c r="I15" s="9" t="n">
         <v>46006</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="57.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="10" t="s">
+      <c r="E16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="85.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="57.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="10" t="s">
+      <c r="E18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="11" t="n">
+      <c r="C19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="9" t="n">
         <v>46034</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="11" t="n">
+      <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I20" s="9" t="n">
         <v>46034</v>
       </c>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" customFormat="false" ht="57.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="57.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G22" s="10" t="s">
+      <c r="E22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="57.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="10" t="s">
+      <c r="E24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="24.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I25" s="11" t="n">
+        <v>110</v>
+      </c>
+      <c r="I25" s="9" t="n">
         <v>46056</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="24.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="43.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="G26" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I26" s="11" t="n">
+        <v>115</v>
+      </c>
+      <c r="I26" s="9" t="n">
         <v>46056</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="24.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G27" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I27" s="11" t="n">
+        <v>80</v>
+      </c>
+      <c r="I27" s="9" t="n">
         <v>46056</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="24.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G28" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I28" s="11" t="n">
+        <v>84</v>
+      </c>
+      <c r="I28" s="9" t="n">
         <v>46056</v>
       </c>
+    </row>
+    <row r="29" customFormat="false" ht="43.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I29" s="9" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="43.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I30" s="9" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I31" s="9" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="57.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I32" s="9" t="n">
+        <v>46065</v>
+      </c>
+      <c r="J32" s="10"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+    </row>
+    <row r="33" customFormat="false" ht="43.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I33" s="9" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="141.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I34" s="9" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="n">
+        <v>35</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="15"/>
+      <c r="I35" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="227.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="n">
+        <v>36</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="97.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="17" t="n">
+        <v>45979</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="108.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I38" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="122.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="14" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="155.35" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I40" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="112.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="14" t="n">
+        <v>38</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="97.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14" t="n">
+        <v>39</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="112.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="14" t="n">
+        <v>38</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I43" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="55.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14" t="n">
+        <v>39</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="14" t="n">
+        <v>38</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="14" t="n">
+        <v>39</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I46" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="20" t="n">
+        <v>40</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="20"/>
+      <c r="I47" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="29.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="20" t="n">
+        <v>40</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="G48" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H48" s="20"/>
+      <c r="I48" s="17" t="n">
+        <v>46065</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>